<commit_message>
#4 update evaluation files
</commit_message>
<xml_diff>
--- a/bernard/experiment/results/results_complete/lcpap_res_stdev.xlsx
+++ b/bernard/experiment/results/results_complete/lcpap_res_stdev.xlsx
@@ -528,19 +528,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="E4" t="n">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="F4" t="n">
-        <v>587</v>
+        <v>264</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -578,19 +578,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2660</v>
+        <v>2662</v>
       </c>
       <c r="C6" t="n">
-        <v>2660</v>
+        <v>2659</v>
       </c>
       <c r="D6" t="n">
-        <v>2633</v>
+        <v>2656</v>
       </c>
       <c r="E6" t="n">
-        <v>2580</v>
+        <v>2649</v>
       </c>
       <c r="F6" t="n">
-        <v>2082</v>
+        <v>2405</v>
       </c>
       <c r="G6" t="n">
         <v>2669</v>
@@ -603,19 +603,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8448275862068966</v>
+        <v>0.875</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8448275862068966</v>
+        <v>0.8305084745762712</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5764705882352941</v>
+        <v>0.7903225806451613</v>
       </c>
       <c r="E7" t="n">
-        <v>0.355072463768116</v>
+        <v>0.7101449275362319</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0770440251572327</v>
+        <v>0.1565495207667732</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
@@ -653,19 +653,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.003372049456725365</v>
+        <v>0.002622705133008617</v>
       </c>
       <c r="C9" t="n">
-        <v>0.003372049456725365</v>
+        <v>0.003746721618583739</v>
       </c>
       <c r="D9" t="n">
-        <v>0.01348819782690146</v>
+        <v>0.004870738104158861</v>
       </c>
       <c r="E9" t="n">
-        <v>0.03334582240539528</v>
+        <v>0.007493443237167478</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2199325590108655</v>
+        <v>0.09891345073061071</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -703,19 +703,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.9074074074074074</v>
+        <v>0.9245283018867924</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9074074074074074</v>
+        <v>0.8990825688073395</v>
       </c>
       <c r="D11" t="n">
-        <v>0.7259259259259259</v>
+        <v>0.8749999999999999</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5212765957446809</v>
+        <v>0.823529411764706</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.2699724517906337</v>
       </c>
       <c r="G11" t="n">
         <v>1</v>
@@ -728,19 +728,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.1551724137931035</v>
+        <v>0.125</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1551724137931035</v>
+        <v>0.1694915254237288</v>
       </c>
       <c r="D12" t="n">
-        <v>0.4235294117647059</v>
+        <v>0.2096774193548387</v>
       </c>
       <c r="E12" t="n">
-        <v>0.644927536231884</v>
+        <v>0.2898550724637681</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9222862799906826</v>
+        <v>0.8434504792332268</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -841,7 +841,7 @@
         <v>46</v>
       </c>
       <c r="F3" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G3" t="n">
         <v>43</v>
@@ -854,19 +854,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="n">
-        <v>115</v>
+        <v>39</v>
       </c>
       <c r="G4" t="n">
         <v>7</v>
@@ -891,7 +891,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5" t="n">
         <v>7</v>
@@ -904,19 +904,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="C6" t="n">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="D6" t="n">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="E6" t="n">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="F6" t="n">
-        <v>1372</v>
+        <v>1448</v>
       </c>
       <c r="G6" t="n">
         <v>1480</v>
@@ -929,19 +929,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8518518518518519</v>
+        <v>0.8363636363636363</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8214285714285714</v>
+        <v>0.7931034482758621</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7419354838709677</v>
+        <v>0.7301587301587301</v>
       </c>
       <c r="E7" t="n">
-        <v>0.647887323943662</v>
+        <v>0.6571428571428571</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2901234567901235</v>
+        <v>0.5411764705882353</v>
       </c>
       <c r="G7" t="n">
         <v>0.86</v>
@@ -966,7 +966,7 @@
         <v>0.92</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.92</v>
       </c>
       <c r="G8" t="n">
         <v>0.86</v>
@@ -979,19 +979,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.005379959650302623</v>
+        <v>0.00605245460659045</v>
       </c>
       <c r="C9" t="n">
-        <v>0.006724949562878279</v>
+        <v>0.008069939475453935</v>
       </c>
       <c r="D9" t="n">
-        <v>0.01075991930060525</v>
+        <v>0.01143241425689307</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0168123739071957</v>
+        <v>0.01613987895090787</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0773369199731002</v>
+        <v>0.02622730329522529</v>
       </c>
       <c r="G9" t="n">
         <v>0.004707464694014795</v>
@@ -1004,19 +1004,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9839139206455951</v>
+        <v>0.9813584398117013</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9857027572293208</v>
+        <v>0.9828648285137862</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9867114996637525</v>
+        <v>0.984034969737727</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9873167451244116</v>
+        <v>0.9852454606590451</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9869132481506389</v>
+        <v>0.985743106926698</v>
       </c>
       <c r="G10" t="n">
         <v>0.9715803631472765</v>
@@ -1029,19 +1029,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.8846153846153846</v>
+        <v>0.8761904761904761</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8679245283018867</v>
+        <v>0.851851851851852</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8214285714285714</v>
+        <v>0.8141592920353983</v>
       </c>
       <c r="E11" t="n">
-        <v>0.7603305785123967</v>
+        <v>0.7666666666666667</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4433962264150944</v>
+        <v>0.6814814814814815</v>
       </c>
       <c r="G11" t="n">
         <v>0.8599999999999999</v>
@@ -1054,19 +1054,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.09626308037737402</v>
+        <v>0.112694660734149</v>
       </c>
       <c r="C12" t="n">
-        <v>0.128539398935325</v>
+        <v>0.1585897644892793</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2128742958125516</v>
+        <v>0.2253683546091777</v>
       </c>
       <c r="E12" t="n">
-        <v>0.3126507935264535</v>
+        <v>0.30283151914826</v>
       </c>
       <c r="F12" t="n">
-        <v>0.6924023520647085</v>
+        <v>0.4145148749154836</v>
       </c>
       <c r="G12" t="n">
         <v>0.09919552426672912</v>
@@ -1155,16 +1155,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3169</v>
+        <v>5164</v>
       </c>
       <c r="C3" t="n">
-        <v>4198</v>
+        <v>6132</v>
       </c>
       <c r="D3" t="n">
-        <v>5987</v>
+        <v>7819</v>
       </c>
       <c r="E3" t="n">
-        <v>8475</v>
+        <v>10541</v>
       </c>
       <c r="F3" t="n">
         <v>14104</v>
@@ -1180,16 +1180,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>358</v>
+        <v>731</v>
       </c>
       <c r="C4" t="n">
-        <v>619</v>
+        <v>946</v>
       </c>
       <c r="D4" t="n">
-        <v>868</v>
+        <v>1542</v>
       </c>
       <c r="E4" t="n">
-        <v>1790</v>
+        <v>2792</v>
       </c>
       <c r="F4" t="n">
         <v>5018</v>
@@ -1205,16 +1205,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>18575</v>
+        <v>16580</v>
       </c>
       <c r="C5" t="n">
-        <v>17546</v>
+        <v>15612</v>
       </c>
       <c r="D5" t="n">
-        <v>15757</v>
+        <v>13925</v>
       </c>
       <c r="E5" t="n">
-        <v>13269</v>
+        <v>11203</v>
       </c>
       <c r="F5" t="n">
         <v>7640</v>
@@ -1230,16 +1230,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>78790</v>
+        <v>78417</v>
       </c>
       <c r="C6" t="n">
-        <v>78529</v>
+        <v>78202</v>
       </c>
       <c r="D6" t="n">
-        <v>78280</v>
+        <v>77606</v>
       </c>
       <c r="E6" t="n">
-        <v>77358</v>
+        <v>76356</v>
       </c>
       <c r="F6" t="n">
         <v>74130</v>
@@ -1255,16 +1255,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.89849730649277</v>
+        <v>0.8759966072943172</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8714967822296035</v>
+        <v>0.8663464255439389</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8733770970094822</v>
+        <v>0.8352740091870526</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8256210423770093</v>
+        <v>0.7905947648691217</v>
       </c>
       <c r="F7" t="n">
         <v>0.7375797510720636</v>
@@ -1280,16 +1280,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1457413539367182</v>
+        <v>0.2374908020603385</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1930647534952171</v>
+        <v>0.2820088300220751</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2753403237674761</v>
+        <v>0.359593451066961</v>
       </c>
       <c r="E8" t="n">
-        <v>0.3897626931567329</v>
+        <v>0.4847774098601913</v>
       </c>
       <c r="F8" t="n">
         <v>0.6486387049300957</v>
@@ -1305,16 +1305,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.004523171779451155</v>
+        <v>0.009235861929549704</v>
       </c>
       <c r="C9" t="n">
-        <v>0.007820791428715824</v>
+        <v>0.01195229190882903</v>
       </c>
       <c r="D9" t="n">
-        <v>0.01096679638146258</v>
+        <v>0.01948248850255218</v>
       </c>
       <c r="E9" t="n">
-        <v>0.02261585889725578</v>
+        <v>0.03527568605650174</v>
       </c>
       <c r="F9" t="n">
         <v>0.06340021226057513</v>
@@ -1330,16 +1330,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.8229706587165825</v>
+        <v>0.877860945871731</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8432738647277837</v>
+        <v>0.8878374291614077</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8671253606241274</v>
+        <v>0.8989298227186497</v>
       </c>
       <c r="E10" t="n">
-        <v>0.8940531151567355</v>
+        <v>0.9118970524403512</v>
       </c>
       <c r="F10" t="n">
         <v>0.9209606058198996</v>
@@ -1355,16 +1355,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.250801313758854</v>
+        <v>0.3736748796989761</v>
       </c>
       <c r="C11" t="n">
-        <v>0.3161025563796543</v>
+        <v>0.4255082922767331</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4186859680408406</v>
+        <v>0.5027487542195788</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5295385672779531</v>
+        <v>0.6010206117969039</v>
       </c>
       <c r="F11" t="n">
         <v>0.6902559584985074</v>
@@ -1380,16 +1380,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.4726945425716088</v>
+        <v>0.3943577370101548</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4305327788137516</v>
+        <v>0.3714723704030001</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3738372879792277</v>
+        <v>0.3378157882265757</v>
       </c>
       <c r="E12" t="n">
-        <v>0.3291134317609947</v>
+        <v>0.3169808092354449</v>
       </c>
       <c r="F12" t="n">
         <v>0.3148738843638855</v>
@@ -1481,16 +1481,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>52</v>
+        <v>477</v>
       </c>
       <c r="C3" t="n">
-        <v>200</v>
+        <v>675</v>
       </c>
       <c r="D3" t="n">
-        <v>368</v>
+        <v>823</v>
       </c>
       <c r="E3" t="n">
-        <v>766</v>
+        <v>852</v>
       </c>
       <c r="F3" t="n">
         <v>916</v>
@@ -1506,16 +1506,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="C4" t="n">
-        <v>25</v>
+        <v>419</v>
       </c>
       <c r="D4" t="n">
-        <v>86</v>
+        <v>657</v>
       </c>
       <c r="E4" t="n">
-        <v>553</v>
+        <v>750</v>
       </c>
       <c r="F4" t="n">
         <v>1093</v>
@@ -1531,16 +1531,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>938</v>
+        <v>513</v>
       </c>
       <c r="C5" t="n">
-        <v>790</v>
+        <v>315</v>
       </c>
       <c r="D5" t="n">
-        <v>622</v>
+        <v>167</v>
       </c>
       <c r="E5" t="n">
-        <v>224</v>
+        <v>138</v>
       </c>
       <c r="F5" t="n">
         <v>74</v>
@@ -1556,16 +1556,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5014</v>
+        <v>4856</v>
       </c>
       <c r="C6" t="n">
-        <v>5004</v>
+        <v>4610</v>
       </c>
       <c r="D6" t="n">
-        <v>4943</v>
+        <v>4372</v>
       </c>
       <c r="E6" t="n">
-        <v>4476</v>
+        <v>4279</v>
       </c>
       <c r="F6" t="n">
         <v>3936</v>
@@ -1581,16 +1581,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.7761194029850746</v>
+        <v>0.7338461538461538</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.6170018281535649</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8105726872246696</v>
+        <v>0.5560810810810811</v>
       </c>
       <c r="E7" t="n">
-        <v>0.5807429871114481</v>
+        <v>0.5318352059925093</v>
       </c>
       <c r="F7" t="n">
         <v>0.4559482329517173</v>
@@ -1606,16 +1606,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.05252525252525252</v>
+        <v>0.4818181818181818</v>
       </c>
       <c r="C8" t="n">
-        <v>0.202020202020202</v>
+        <v>0.6818181818181818</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3717171717171717</v>
+        <v>0.8313131313131313</v>
       </c>
       <c r="E8" t="n">
-        <v>0.7737373737373737</v>
+        <v>0.8606060606060606</v>
       </c>
       <c r="F8" t="n">
         <v>0.9252525252525252</v>
@@ -1631,16 +1631,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.002982700338039372</v>
+        <v>0.03440047723205408</v>
       </c>
       <c r="C9" t="n">
-        <v>0.00497116723006562</v>
+        <v>0.08331676277589978</v>
       </c>
       <c r="D9" t="n">
-        <v>0.01710081527142573</v>
+        <v>0.1306422748061245</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1099622191290515</v>
+        <v>0.1491350169019686</v>
       </c>
       <c r="F9" t="n">
         <v>0.2173394312984689</v>
@@ -1656,16 +1656,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9284744441833326</v>
+        <v>0.9206328546952925</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9285780854880078</v>
+        <v>0.9238794788208189</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9285170254945557</v>
+        <v>0.9261640063389915</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9286240813383386</v>
+        <v>0.9277079805813152</v>
       </c>
       <c r="F10" t="n">
         <v>0.9285559914114299</v>
@@ -1681,16 +1681,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.09839167455061494</v>
+        <v>0.5817073170731707</v>
       </c>
       <c r="C11" t="n">
-        <v>0.3292181069958848</v>
+        <v>0.647792706333973</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5096952908587258</v>
+        <v>0.6663967611336034</v>
       </c>
       <c r="E11" t="n">
-        <v>0.6634906886097878</v>
+        <v>0.6574074074074073</v>
       </c>
       <c r="F11" t="n">
         <v>0.6108702900966988</v>
@@ -1706,16 +1706,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.614032009733704</v>
+        <v>0.3826588842117208</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5193301082183785</v>
+        <v>0.3932478192219317</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3963127909250077</v>
+        <v>0.399826471407318</v>
       </c>
       <c r="E12" t="n">
-        <v>0.3931878849412639</v>
+        <v>0.4257248017392865</v>
       </c>
       <c r="F12" t="n">
         <v>0.5225807672735745</v>
@@ -1807,16 +1807,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>321</v>
       </c>
       <c r="C3" t="n">
-        <v>16</v>
+        <v>421</v>
       </c>
       <c r="D3" t="n">
-        <v>100</v>
+        <v>711</v>
       </c>
       <c r="E3" t="n">
-        <v>372</v>
+        <v>822</v>
       </c>
       <c r="F3" t="n">
         <v>863</v>
@@ -1832,16 +1832,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="C4" t="n">
-        <v>26</v>
+        <v>195</v>
       </c>
       <c r="D4" t="n">
-        <v>60</v>
+        <v>592</v>
       </c>
       <c r="E4" t="n">
-        <v>166</v>
+        <v>900</v>
       </c>
       <c r="F4" t="n">
         <v>1230</v>
@@ -1857,16 +1857,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>985</v>
+        <v>669</v>
       </c>
       <c r="C5" t="n">
-        <v>974</v>
+        <v>569</v>
       </c>
       <c r="D5" t="n">
-        <v>890</v>
+        <v>279</v>
       </c>
       <c r="E5" t="n">
-        <v>618</v>
+        <v>168</v>
       </c>
       <c r="F5" t="n">
         <v>127</v>
@@ -1882,16 +1882,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5012</v>
+        <v>4931</v>
       </c>
       <c r="C6" t="n">
-        <v>5003</v>
+        <v>4834</v>
       </c>
       <c r="D6" t="n">
-        <v>4969</v>
+        <v>4437</v>
       </c>
       <c r="E6" t="n">
-        <v>4863</v>
+        <v>4129</v>
       </c>
       <c r="F6" t="n">
         <v>3799</v>
@@ -1907,16 +1907,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2272727272727273</v>
+        <v>0.766109785202864</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3809523809523809</v>
+        <v>0.6834415584415584</v>
       </c>
       <c r="D7" t="n">
-        <v>0.625</v>
+        <v>0.545663852647736</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6914498141263941</v>
+        <v>0.4773519163763066</v>
       </c>
       <c r="F7" t="n">
         <v>0.4123268036311515</v>
@@ -1932,16 +1932,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.005050505050505051</v>
+        <v>0.3242424242424242</v>
       </c>
       <c r="C8" t="n">
-        <v>0.01616161616161616</v>
+        <v>0.4252525252525253</v>
       </c>
       <c r="D8" t="n">
-        <v>0.101010101010101</v>
+        <v>0.7181818181818181</v>
       </c>
       <c r="E8" t="n">
-        <v>0.3757575757575757</v>
+        <v>0.8303030303030303</v>
       </c>
       <c r="F8" t="n">
         <v>0.8717171717171717</v>
@@ -1957,16 +1957,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.003380393716444621</v>
+        <v>0.01948697554185723</v>
       </c>
       <c r="C9" t="n">
-        <v>0.005170013919268244</v>
+        <v>0.03877510439451183</v>
       </c>
       <c r="D9" t="n">
-        <v>0.01193080135215749</v>
+        <v>0.1177172400079539</v>
       </c>
       <c r="E9" t="n">
-        <v>0.03300855040763571</v>
+        <v>0.1789620202823623</v>
       </c>
       <c r="F9" t="n">
         <v>0.2445814277192285</v>
@@ -1982,16 +1982,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.8867335112910775</v>
+        <v>0.8687190055255277</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8862390056862121</v>
+        <v>0.8738637116843521</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8857736240913812</v>
+        <v>0.8786217715030601</v>
       </c>
       <c r="E10" t="n">
-        <v>0.8848193608384501</v>
+        <v>0.8829146505821788</v>
       </c>
       <c r="F10" t="n">
         <v>0.8840623374327889</v>
@@ -2007,16 +2007,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.009881422924901186</v>
+        <v>0.4556422995031937</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0310077519379845</v>
+        <v>0.5242839352428393</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1739130434782609</v>
+        <v>0.6201482773658962</v>
       </c>
       <c r="E11" t="n">
-        <v>0.4869109947643979</v>
+        <v>0.6061946902654868</v>
       </c>
       <c r="F11" t="n">
         <v>0.559844307492702</v>
@@ -2032,16 +2032,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.7114820200428496</v>
+        <v>0.4377928471364327</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6754370860911674</v>
+        <v>0.4175659788130125</v>
       </c>
       <c r="D12" t="n">
-        <v>0.571976520383579</v>
+        <v>0.4301611845145062</v>
       </c>
       <c r="E12" t="n">
-        <v>0.443548070635101</v>
+        <v>0.4780397609556685</v>
       </c>
       <c r="F12" t="n">
         <v>0.5539006224610462</v>
@@ -2133,16 +2133,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>294</v>
       </c>
       <c r="C3" t="n">
-        <v>13</v>
+        <v>378</v>
       </c>
       <c r="D3" t="n">
-        <v>87</v>
+        <v>667</v>
       </c>
       <c r="E3" t="n">
-        <v>347</v>
+        <v>818</v>
       </c>
       <c r="F3" t="n">
         <v>861</v>
@@ -2158,16 +2158,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="C4" t="n">
-        <v>26</v>
+        <v>173</v>
       </c>
       <c r="D4" t="n">
-        <v>62</v>
+        <v>568</v>
       </c>
       <c r="E4" t="n">
-        <v>165</v>
+        <v>927</v>
       </c>
       <c r="F4" t="n">
         <v>1274</v>
@@ -2183,16 +2183,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>985</v>
+        <v>696</v>
       </c>
       <c r="C5" t="n">
-        <v>977</v>
+        <v>612</v>
       </c>
       <c r="D5" t="n">
-        <v>903</v>
+        <v>323</v>
       </c>
       <c r="E5" t="n">
-        <v>643</v>
+        <v>172</v>
       </c>
       <c r="F5" t="n">
         <v>129</v>
@@ -2208,16 +2208,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5012</v>
+        <v>4939</v>
       </c>
       <c r="C6" t="n">
-        <v>5003</v>
+        <v>4856</v>
       </c>
       <c r="D6" t="n">
-        <v>4967</v>
+        <v>4461</v>
       </c>
       <c r="E6" t="n">
-        <v>4864</v>
+        <v>4102</v>
       </c>
       <c r="F6" t="n">
         <v>3755</v>
@@ -2233,16 +2233,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2272727272727273</v>
+        <v>0.765625</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.6860254083484574</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5838926174496645</v>
+        <v>0.540080971659919</v>
       </c>
       <c r="E7" t="n">
-        <v>0.677734375</v>
+        <v>0.4687679083094556</v>
       </c>
       <c r="F7" t="n">
         <v>0.4032786885245901</v>
@@ -2258,16 +2258,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.005050505050505051</v>
+        <v>0.296969696969697</v>
       </c>
       <c r="C8" t="n">
-        <v>0.01313131313131313</v>
+        <v>0.3818181818181818</v>
       </c>
       <c r="D8" t="n">
-        <v>0.08787878787878788</v>
+        <v>0.6737373737373737</v>
       </c>
       <c r="E8" t="n">
-        <v>0.3505050505050505</v>
+        <v>0.8262626262626263</v>
       </c>
       <c r="F8" t="n">
         <v>0.8696969696969697</v>
@@ -2283,16 +2283,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.003380393716444621</v>
+        <v>0.01789620202823623</v>
       </c>
       <c r="C9" t="n">
-        <v>0.005170013919268244</v>
+        <v>0.03440047723205408</v>
       </c>
       <c r="D9" t="n">
-        <v>0.01232849473056274</v>
+        <v>0.1129449194670909</v>
       </c>
       <c r="E9" t="n">
-        <v>0.03280970371843309</v>
+        <v>0.1843308808908332</v>
       </c>
       <c r="F9" t="n">
         <v>0.2533306820441439</v>
@@ -2308,16 +2308,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.8767070184847078</v>
+        <v>0.8591347959612028</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8762530856386493</v>
+        <v>0.8642634337006975</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8759578284334697</v>
+        <v>0.8688314844608342</v>
       </c>
       <c r="E10" t="n">
-        <v>0.8752128563423056</v>
+        <v>0.872502716567143</v>
       </c>
       <c r="F10" t="n">
         <v>0.874570320424367</v>
@@ -2333,16 +2333,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.009881422924901186</v>
+        <v>0.4279475982532752</v>
       </c>
       <c r="C11" t="n">
-        <v>0.02526724975704568</v>
+        <v>0.4905905256327061</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1527655838454785</v>
+        <v>0.5995505617977528</v>
       </c>
       <c r="E11" t="n">
-        <v>0.4620505992010653</v>
+        <v>0.5981718464351006</v>
       </c>
       <c r="F11" t="n">
         <v>0.55104</v>
@@ -2358,16 +2358,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.7114820200428496</v>
+        <v>0.4485691815869852</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6662173582652207</v>
+        <v>0.432995291059961</v>
       </c>
       <c r="D12" t="n">
-        <v>0.6004568006953032</v>
+        <v>0.4377121777903288</v>
       </c>
       <c r="E12" t="n">
-        <v>0.4622989855575607</v>
+        <v>0.4867551084873004</v>
       </c>
       <c r="F12" t="n">
         <v>0.5633289538315495</v>
@@ -2459,16 +2459,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>189</v>
       </c>
       <c r="C3" t="n">
-        <v>7</v>
+        <v>316</v>
       </c>
       <c r="D3" t="n">
-        <v>62</v>
+        <v>505</v>
       </c>
       <c r="E3" t="n">
-        <v>249</v>
+        <v>798</v>
       </c>
       <c r="F3" t="n">
         <v>853</v>
@@ -2484,16 +2484,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="C4" t="n">
-        <v>27</v>
+        <v>165</v>
       </c>
       <c r="D4" t="n">
-        <v>63</v>
+        <v>427</v>
       </c>
       <c r="E4" t="n">
-        <v>159</v>
+        <v>973</v>
       </c>
       <c r="F4" t="n">
         <v>1464</v>
@@ -2509,16 +2509,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>987</v>
+        <v>801</v>
       </c>
       <c r="C5" t="n">
-        <v>983</v>
+        <v>674</v>
       </c>
       <c r="D5" t="n">
-        <v>928</v>
+        <v>485</v>
       </c>
       <c r="E5" t="n">
-        <v>741</v>
+        <v>192</v>
       </c>
       <c r="F5" t="n">
         <v>137</v>
@@ -2534,16 +2534,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5012</v>
+        <v>4938</v>
       </c>
       <c r="C6" t="n">
-        <v>5002</v>
+        <v>4864</v>
       </c>
       <c r="D6" t="n">
-        <v>4966</v>
+        <v>4602</v>
       </c>
       <c r="E6" t="n">
-        <v>4870</v>
+        <v>4056</v>
       </c>
       <c r="F6" t="n">
         <v>3565</v>
@@ -2559,16 +2559,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.15</v>
+        <v>0.675</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2058823529411765</v>
+        <v>0.656964656964657</v>
       </c>
       <c r="D7" t="n">
-        <v>0.496</v>
+        <v>0.5418454935622318</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6102941176470589</v>
+        <v>0.4505928853754941</v>
       </c>
       <c r="F7" t="n">
         <v>0.368148467846353</v>
@@ -2584,16 +2584,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.00303030303030303</v>
+        <v>0.1909090909090909</v>
       </c>
       <c r="C8" t="n">
-        <v>0.007070707070707071</v>
+        <v>0.3191919191919192</v>
       </c>
       <c r="D8" t="n">
-        <v>0.06262626262626263</v>
+        <v>0.5101010101010101</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2515151515151515</v>
+        <v>0.806060606060606</v>
       </c>
       <c r="F8" t="n">
         <v>0.8616161616161616</v>
@@ -2609,16 +2609,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.003380393716444621</v>
+        <v>0.01809504871743885</v>
       </c>
       <c r="C9" t="n">
-        <v>0.005368860608470869</v>
+        <v>0.03280970371843309</v>
       </c>
       <c r="D9" t="n">
-        <v>0.01252734141976536</v>
+        <v>0.08490753628952077</v>
       </c>
       <c r="E9" t="n">
-        <v>0.03161662358321734</v>
+        <v>0.1934778285941539</v>
       </c>
       <c r="F9" t="n">
         <v>0.2911115529926427</v>
@@ -2634,16 +2634,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.8512048301668504</v>
+        <v>0.8348409527769241</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8509180088818189</v>
+        <v>0.8403142581110368</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8504911914933787</v>
+        <v>0.8442576490697389</v>
       </c>
       <c r="E10" t="n">
-        <v>0.8498868180713477</v>
+        <v>0.848517186178749</v>
       </c>
       <c r="F10" t="n">
         <v>0.8494923383768085</v>
@@ -2659,16 +2659,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.005940594059405942</v>
+        <v>0.2976377952755905</v>
       </c>
       <c r="C11" t="n">
-        <v>0.013671875</v>
+        <v>0.4296397008837525</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1112107623318386</v>
+        <v>0.5254942767950052</v>
       </c>
       <c r="E11" t="n">
-        <v>0.3562231759656653</v>
+        <v>0.5780514306410721</v>
       </c>
       <c r="F11" t="n">
         <v>0.5158754157846991</v>
@@ -2684,16 +2684,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.7146245333110881</v>
+        <v>0.5448595481843249</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6944974475621293</v>
+        <v>0.4692436449299321</v>
       </c>
       <c r="D12" t="n">
-        <v>0.6108406302131797</v>
+        <v>0.4678375239905984</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5289383085869971</v>
+        <v>0.5027841163096147</v>
       </c>
       <c r="F12" t="n">
         <v>0.5995831475287997</v>

</xml_diff>